<commit_message>
dOx: Gameboard Header finished Gameboard.h: delete of unused method bool checkGameOver() Gameboard.cpp: ~Gameboard, now calling removeAllItems() setLevel(int level): added delete currentLevel, check if lagging error is now resolved 😊 it's solved on my side
</commit_message>
<xml_diff>
--- a/Administration/Répartition.xlsx
+++ b/Administration/Répartition.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Téléchargements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rocla/Clouds/OneDrive/HE-Arc/Projet Qt/P2ete/Administration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26200" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>PHASE 1</t>
   </si>
@@ -57,6 +60,12 @@
   </si>
   <si>
     <t>Romain</t>
+  </si>
+  <si>
+    <t>Factory Characters</t>
+  </si>
+  <si>
+    <t>Factory Surfaces</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +170,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -233,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,23 +392,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -407,7 +416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -415,17 +424,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -433,17 +448,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Début de réparation du premier dialog - Ajout du commentaire de classe pour G_Level
</commit_message>
<xml_diff>
--- a/Administration/Répartition.xlsx
+++ b/Administration/Répartition.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rocla/Clouds/OneDrive/HE-Arc/Projet Qt/P2ete/Administration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\P2 Summer\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26200" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="26205" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -72,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +82,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,20 +404,20 @@
   <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -416,15 +425,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -432,7 +441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -440,7 +449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -448,12 +457,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -461,7 +470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -469,11 +478,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correction des fichiers administratifs Ajout des éléments pour les menus
</commit_message>
<xml_diff>
--- a/Administration/Répartition.xlsx
+++ b/Administration/Répartition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>PHASE 1</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>Factory Surfaces</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Graphisme</t>
+  </si>
+  <si>
+    <t>Capacités spéciales (Decorator)</t>
+  </si>
+  <si>
+    <t>Déplacement de blocs</t>
+  </si>
+  <si>
+    <t>Menu pause amélioré</t>
+  </si>
+  <si>
+    <t>Eviter les messages infos du tuto</t>
+  </si>
+  <si>
+    <t>Interaction avec les acteurs (loutre)</t>
+  </si>
+  <si>
+    <t>Crédits du jeu</t>
   </si>
 </sst>
 </file>
@@ -401,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +510,52 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout de quelques musiques
</commit_message>
<xml_diff>
--- a/Administration/Répartition.xlsx
+++ b/Administration/Répartition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>PHASE 1</t>
   </si>
@@ -35,68 +35,65 @@
     <t xml:space="preserve">Test Bench </t>
   </si>
   <si>
-    <t>Génération des cartes</t>
-  </si>
-  <si>
-    <t>Fusion Personnages/Ennemis</t>
-  </si>
-  <si>
-    <t>Ennemis (State/Observer)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Champ de détection </t>
-  </si>
-  <si>
     <t>Thread pour les ennemis</t>
   </si>
   <si>
-    <t>dOxygen</t>
-  </si>
-  <si>
     <t>Steve</t>
   </si>
   <si>
-    <t>Margaux</t>
-  </si>
-  <si>
     <t>Romain</t>
   </si>
   <si>
-    <t>Factory Characters</t>
-  </si>
-  <si>
-    <t>Factory Surfaces</t>
-  </si>
-  <si>
     <t>Son</t>
   </si>
   <si>
-    <t>Graphisme</t>
-  </si>
-  <si>
     <t>Capacités spéciales (Decorator)</t>
   </si>
   <si>
     <t>Déplacement de blocs</t>
   </si>
   <si>
-    <t>Menu pause amélioré</t>
-  </si>
-  <si>
-    <t>Eviter les messages infos du tuto</t>
-  </si>
-  <si>
     <t>Interaction avec les acteurs (loutre)</t>
   </si>
   <si>
-    <t>Crédits du jeu</t>
+    <t>(Evt)</t>
+  </si>
+  <si>
+    <t>Graphisme / Animation</t>
+  </si>
+  <si>
+    <t>Création des ennemis et des niveaux</t>
+  </si>
+  <si>
+    <t>Amélioration de l'histoire (Animations infos)</t>
+  </si>
+  <si>
+    <t>Coffres et lieux secrets</t>
+  </si>
+  <si>
+    <t>Trace de pas du pingouin dans la neige + Détection</t>
+  </si>
+  <si>
+    <t>Déplacements intelligents des ennemis (IA)</t>
+  </si>
+  <si>
+    <t>Champ de vision du pingouin perturbé (Brume, Luminosité)</t>
+  </si>
+  <si>
+    <t>Niveau de difficulté haute</t>
+  </si>
+  <si>
+    <t>Classement des meilleurs temps obtenus</t>
+  </si>
+  <si>
+    <t>Générateur de maps pour les utilisateurs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,14 +103,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,10 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,113 +413,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -549,11 +519,6 @@
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout du boss *Walrus" Ajout de l'état pour envoyer des blocs Ajout des dialogues plus personnalisés ...
</commit_message>
<xml_diff>
--- a/Administration/Répartition.xlsx
+++ b/Administration/Répartition.xlsx
@@ -130,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +417,7 @@
   <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,9 +463,11 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">

</xml_diff>